<commit_message>
Add data to excel file
</commit_message>
<xml_diff>
--- a/Team_project_ template.xlsx
+++ b/Team_project_ template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\dss\week5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\dss\week5\teamdowns\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
   <si>
     <t>xx1</t>
   </si>
@@ -390,6 +390,9 @@
   </si>
   <si>
     <t>서울 중구 신당동</t>
+  </si>
+  <si>
+    <t>종로 신설동역한양립스</t>
   </si>
 </sst>
 </file>
@@ -894,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R53"/>
+  <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25"/>
@@ -1566,7 +1569,7 @@
         <v>7</v>
       </c>
       <c r="G14">
-        <f t="shared" ref="G14:G52" si="1">3.305785*F14</f>
+        <f t="shared" ref="G14:G53" si="1">3.305785*F14</f>
         <v>23.140495000000001</v>
       </c>
       <c r="H14">
@@ -1811,7 +1814,7 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <f t="shared" ref="O18:O52" si="2">(P18+Q18)*100+R18</f>
+        <f t="shared" ref="O18:O53" si="2">(P18+Q18)*100+R18</f>
         <v>4800</v>
       </c>
       <c r="P18" s="7">
@@ -3606,7 +3609,61 @@
       </c>
     </row>
     <row r="53" spans="2:18">
-      <c r="F53" s="16"/>
+      <c r="D53" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F53" s="16">
+        <v>5</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="1"/>
+        <v>16.528925000000001</v>
+      </c>
+      <c r="H53">
+        <v>11</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53" s="7">
+        <v>1</v>
+      </c>
+      <c r="K53" s="7">
+        <v>1</v>
+      </c>
+      <c r="L53" s="7">
+        <v>1</v>
+      </c>
+      <c r="M53" s="7">
+        <v>1</v>
+      </c>
+      <c r="N53" s="7">
+        <v>1</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="2"/>
+        <v>7200</v>
+      </c>
+      <c r="P53" s="7">
+        <v>7</v>
+      </c>
+      <c r="Q53" s="7">
+        <v>60</v>
+      </c>
+      <c r="R53">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="54" spans="2:18">
+      <c r="D54" s="10"/>
+      <c r="H54">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="2:18">
+      <c r="H56">
+        <v>4.45</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>